<commit_message>
First implementation with multiple AI providers
</commit_message>
<xml_diff>
--- a/test-files/Book1.xlsx
+++ b/test-files/Book1.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas.alberti/otherRepos/go-excel-ai/test-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D887939-6A23-484F-9C72-03762DC4E7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nelle zone di quota di maggior afflusso turistico ed escursionistico la
 frequentazione antropica sia invernale che estiva, quando è
@@ -101,12 +100,21 @@
   <si>
     <t>L'obiettivo principale di questa azione è la conservazione e il mantenimento dei pascoli tradizionalmente monticati con bovini all'interno dell'ATO Monte Bondone, in particolare nelle zone di Val d'Eva, Le Coe, bassa Val del Merlo, Viote, Brigolina, Malghet, Dosso della Croce, Montesel, I Colmi, Malga Albi. Queste aree sono caratterizzate da elevati livelli di biodiversità e l'obiettivo è prevenire l'abbandono del territorio. Inoltre, l'azione mira a mantenere i prati aridi sui Dossi di Omalga, Sopramonte e in generale in tutte le aree dove non è possibile effettuare uno sfalcio con cadenza biennale. I pascoli di quota e le praterie aride sono elementi distintivi del territorio, risultato dei disboscamenti avvenuti nei secoli passati. Questi habitat sono importanti per numerose specie floristiche e rappresentano luoghi di nidificazione e alimentazione per diverse specie di uccelli tipiche delle zone aperte. La tendenza attuale verso la ricolonizzazione degli ambienti aperti da parte degli arbusti, a causa dell'abbandono delle pratiche agricole tradizionali, sta portando a una diminuzione della diversità territoriale e delle specie presenti. Per contrastare questa tendenza, è necessario incentivare un pascolamento regolare ed estensivo. La regolamentazione del pascolo interrompe la naturale tendenza al ritorno del bosco, favorendo le specie legate agli ambienti aperti e aumentando la disponibilità di prede per l'ornitofauna.</t>
   </si>
+  <si>
+    <t>OpenAI response to 'Prova di un prompt'</t>
+  </si>
+  <si>
+    <t>OpenAI response to 'Prova di un prompt SALVATO'</t>
+  </si>
+  <si>
+    <t>Ollama (llama3.1) response to 'Prova di un prompt SALVATO'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,18 +145,18 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -161,7 +169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -479,25 +487,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDE2CA0-0BD9-BE42-932C-70B94D0C11E1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="76" customWidth="1"/>
-    <col min="2" max="2" width="64.83203125" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="76"/>
+    <col customWidth="true" max="2" min="2" width="64.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="119">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="409.6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>